<commit_message>
updated adj study calculated mean and sd
</commit_message>
<xml_diff>
--- a/ptg effect sizes.xlsx
+++ b/ptg effect sizes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="46">
   <si>
     <t xml:space="preserve">study name</t>
   </si>
@@ -46,21 +46,21 @@
     <t xml:space="preserve">PTGI-SF</t>
   </si>
   <si>
+    <t xml:space="preserve">this is correct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arnout 2021 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTGI</t>
+  </si>
+  <si>
     <t xml:space="preserve">need to average male and female </t>
   </si>
   <si>
-    <t xml:space="preserve">Arnout 2021 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PTG-21</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chasson 2022</t>
   </si>
   <si>
-    <t xml:space="preserve">PTGI</t>
-  </si>
-  <si>
     <t xml:space="preserve">need to average the jews and the arbs </t>
   </si>
   <si>
@@ -88,18 +88,12 @@
     <t xml:space="preserve">Feingold 2022</t>
   </si>
   <si>
-    <t xml:space="preserve">90% has positive change</t>
-  </si>
-  <si>
     <t xml:space="preserve">needs to email author about the descriptives; high confidence to get a response</t>
   </si>
   <si>
     <t xml:space="preserve">Gul 2023</t>
   </si>
   <si>
-    <t xml:space="preserve">this is correct</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kalaizaki 2022</t>
   </si>
   <si>
@@ -122,9 +116,6 @@
   </si>
   <si>
     <t xml:space="preserve">Pirtrzak 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43.3% indicated they have experience PTG</t>
   </si>
   <si>
     <t xml:space="preserve">need to convert this into a common scale</t>
@@ -340,10 +331,10 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.47"/>
@@ -380,7 +371,10 @@
         <v>7</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>23.1</v>
+        <v>22.258</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>5.052</v>
       </c>
       <c r="E2" s="0" t="n">
         <f aca="false">226 + 155</f>
@@ -405,15 +399,15 @@
         <v>365</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" s="0" t="n">
         <f aca="false">2.91*21</f>
@@ -432,7 +426,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" s="0" t="n">
         <f aca="false">38.09 * 10.7/100 + 73.78 * 20.1/100 + 57.91 * 42.2/100 + 79.47 * 27/100</f>
@@ -489,22 +483,19 @@
       <c r="B8" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>22</v>
-      </c>
       <c r="E8" s="0" t="n">
         <v>787</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>45.57</v>
@@ -516,15 +507,15 @@
         <v>300</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>47.73</v>
@@ -533,15 +524,15 @@
         <v>352</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>35</v>
@@ -550,12 +541,12 @@
         <v>327</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>7</v>
@@ -563,19 +554,22 @@
       <c r="C12" s="0" t="n">
         <v>12.64</v>
       </c>
+      <c r="D12" s="0" t="n">
+        <v>11.01</v>
+      </c>
       <c r="E12" s="0" t="n">
         <v>1424</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">2.9*21</f>
@@ -585,15 +579,15 @@
         <v>401</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>96.26</v>
@@ -602,15 +596,15 @@
         <v>266</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>47</v>
@@ -619,32 +613,29 @@
         <v>296</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="0" t="s">
-        <v>34</v>
-      </c>
       <c r="E16" s="0" t="n">
         <v>395</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>3.25</v>
@@ -656,12 +647,12 @@
         <v>1492</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>7</v>
@@ -673,12 +664,12 @@
         <v>12686</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>7</v>
@@ -690,15 +681,15 @@
         <v>1951</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>46</v>
@@ -707,12 +698,12 @@
         <v>193</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>7</v>
@@ -727,15 +718,15 @@
         <v>1510</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>63.49</v>
@@ -744,15 +735,15 @@
         <v>292</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>21.658</v>
@@ -764,15 +755,15 @@
         <v>423</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>67.17</v>
@@ -784,15 +775,15 @@
         <v>1790</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>58.34</v>
@@ -804,7 +795,7 @@
         <v>442</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
update ptg effect sizes
</commit_message>
<xml_diff>
--- a/ptg effect sizes.xlsx
+++ b/ptg effect sizes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="43">
   <si>
     <t xml:space="preserve">study name</t>
   </si>
@@ -55,27 +55,15 @@
     <t xml:space="preserve">PTGI</t>
   </si>
   <si>
-    <t xml:space="preserve">need to average male and female </t>
-  </si>
-  <si>
     <t xml:space="preserve">Chasson 2022</t>
   </si>
   <si>
-    <t xml:space="preserve">need to average the jews and the arbs </t>
+    <t xml:space="preserve">Chen 2022</t>
   </si>
   <si>
     <t xml:space="preserve">Chen 2021</t>
   </si>
   <si>
-    <t xml:space="preserve">this one is corrected calculated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chen 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">need to double check on this one later</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dominick 2023</t>
   </si>
   <si>
@@ -88,7 +76,7 @@
     <t xml:space="preserve">Feingold 2022</t>
   </si>
   <si>
-    <t xml:space="preserve">needs to email author about the descriptives; high confidence to get a response</t>
+    <t xml:space="preserve">this study has everything but the descriptives we need </t>
   </si>
   <si>
     <t xml:space="preserve">Gul 2023</t>
@@ -103,10 +91,13 @@
     <t xml:space="preserve">Lewis 2021</t>
   </si>
   <si>
-    <t xml:space="preserve">Lyu 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">double check on the sample size later </t>
+    <t xml:space="preserve">Lyu 2021a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this is correct; select time 2; all things considered, study 2 is probably better for our purposes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lyu 2021b</t>
   </si>
   <si>
     <t xml:space="preserve">Mo 2022</t>
@@ -115,10 +106,10 @@
     <t xml:space="preserve">Northfield 2022</t>
   </si>
   <si>
-    <t xml:space="preserve">Pirtrzak 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">need to convert this into a common scale</t>
+    <t xml:space="preserve">Pietrzak 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this study does not have viable effect sizes</t>
   </si>
   <si>
     <t xml:space="preserve">Prieto 2020</t>
@@ -133,16 +124,16 @@
     <t xml:space="preserve">Ulset 2021</t>
   </si>
   <si>
+    <t xml:space="preserve">Vazquez 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Willey 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yeung 2022</t>
+  </si>
+  <si>
     <t xml:space="preserve">need to find a good multiplier for this one </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vazquez 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Willey 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yeung 2022</t>
   </si>
   <si>
     <t xml:space="preserve">Yildiz 2021</t>
@@ -190,12 +181,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFBF00"/>
+        <bgColor rgb="FFFF8000"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -238,7 +235,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -247,7 +244,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -305,7 +306,7 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFFBF00"/>
       <rgbColor rgb="FFFF8000"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
@@ -331,7 +332,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -392,38 +393,43 @@
         <v>10</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>67.5</v>
+        <v>65.195</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>5.052</v>
       </c>
       <c r="E3" s="0" t="n">
         <f aca="false">94+141+84+46</f>
         <v>365</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="0" t="n">
-        <f aca="false">2.91*21</f>
-        <v>61.11</v>
+        <v>55.78</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>19.1</v>
       </c>
       <c r="E4" s="0" t="n">
         <f aca="false">517+399</f>
         <v>916</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>10</v>
@@ -433,18 +439,18 @@
         <v>64.80033</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>10.44373</v>
+        <v>10.44</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>422</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>7</v>
@@ -452,19 +458,22 @@
       <c r="C6" s="0" t="n">
         <v>28</v>
       </c>
+      <c r="D6" s="0" t="n">
+        <v>11.5</v>
+      </c>
       <c r="E6" s="0" t="n">
         <v>12596</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>1.39</v>
@@ -473,26 +482,27 @@
         <v>201</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="n">
         <v>787</v>
       </c>
-      <c r="F8" s="0" t="s">
-        <v>22</v>
+      <c r="F8" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>10</v>
@@ -512,7 +522,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>10</v>
@@ -520,6 +530,9 @@
       <c r="C10" s="0" t="n">
         <v>47.73</v>
       </c>
+      <c r="D10" s="0" t="n">
+        <v>24.63</v>
+      </c>
       <c r="E10" s="0" t="n">
         <v>352</v>
       </c>
@@ -529,15 +542,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>35</v>
+        <v>53.13</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>17.22</v>
       </c>
       <c r="E11" s="0" t="n">
+        <f aca="false"> 235 + 92</f>
         <v>327</v>
       </c>
       <c r="F11" s="0" t="s">
@@ -546,7 +563,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>7</v>
@@ -566,34 +583,39 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="0" t="n">
-        <f aca="false">2.9*21</f>
-        <v>60.9</v>
+        <v>78.4</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>14</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>401</v>
+        <v>251</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>96.26</v>
+        <v>58.8</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>14.8</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>266</v>
+        <v>401</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>8</v>
@@ -601,16 +623,19 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>47</v>
+        <v>96.26</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>21.57</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>296</v>
+        <v>266</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>8</v>
@@ -618,67 +643,74 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>28.2</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>296</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="n">
+        <v>395</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="0" t="n">
-        <v>395</v>
-      </c>
-      <c r="F16" s="0" t="s">
+      <c r="C18" s="2" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>1492</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="17" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="1" t="n">
-        <v>3.25</v>
-      </c>
-      <c r="D17" s="1" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="E17" s="1" t="n">
-        <v>1492</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="0" t="n">
-        <v>2.16</v>
-      </c>
-      <c r="E18" s="0" t="n">
-        <v>12686</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>36.51</v>
+        <v>21.6</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>6.8</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>1951</v>
+        <v>12686</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>8</v>
@@ -686,16 +718,19 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>46</v>
+        <v>36.51</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>7.6</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>193</v>
+        <v>1951</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>8</v>
@@ -703,105 +738,122 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>2.19</v>
+        <v>47.95</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>0.97</v>
+        <v>24.48</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>1510</v>
+        <v>176</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C22" s="0" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>1510</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="0" t="n">
         <v>63.49</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="D23" s="0" t="n">
+        <v>20.64</v>
+      </c>
+      <c r="E23" s="0" t="n">
         <v>292</v>
       </c>
-      <c r="F22" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="1" t="n">
+      <c r="F23" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="2" t="n">
         <v>21.658</v>
       </c>
-      <c r="D23" s="1" t="n">
+      <c r="D24" s="2" t="n">
         <v>4.615</v>
       </c>
-      <c r="E23" s="1" t="n">
+      <c r="E24" s="2" t="n">
         <v>423</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="0" t="n">
-        <v>67.17</v>
-      </c>
-      <c r="D24" s="0" t="n">
-        <v>14.79</v>
-      </c>
-      <c r="E24" s="0" t="n">
-        <v>1790</v>
-      </c>
-      <c r="F24" s="0" t="s">
+      <c r="F24" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>10</v>
       </c>
       <c r="C25" s="0" t="n">
+        <v>67.17</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>14.79</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>1790</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="0" t="n">
         <v>58.34</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D26" s="0" t="n">
         <v>26.76</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E26" s="0" t="n">
         <v>442</v>
       </c>
-      <c r="F25" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E26" s="0" t="n">
-        <f aca="false">SUM(E2:E25)</f>
-        <v>40208</v>
+      <c r="F26" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>